<commit_message>
commiting proj files for GH action?
</commit_message>
<xml_diff>
--- a/project/excel/mifc.xlsx
+++ b/project/excel/mifc.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Food" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Component" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Container" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Provenance" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Container" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,91 +427,147 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_food_type</t>
+          <t>food_primary_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>primary_food_type_label</t>
+          <t>food_primary_type_label</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>primary_food_type_upc_code</t>
+          <t>food_upc_code</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>food_preparation_state</t>
+          <t>food_preservation_state</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>food_storage_temperature_state</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>food_ripeness_state</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>food_cooking_method</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>food_acquisition_city</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>food_acquisition_country</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>food_acquisition_country_subdivision</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>food_acquisition_date</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>food_acquisition_location_type</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>food_acquisition_latitude</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>food_acquisition_longitude</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>food_acquisition_agent_name</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>food_acquisition_organization</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
         <is>
           <t>food_distributor_city</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>food_distributor_country</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>food_distributor_country_subdivision</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>food_expiration_date</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>food_category_label</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>food_additional_types</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_id</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_aliquot_id</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_batch_id</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"raw,fresh,chilled,foodsafe chilled,fresh chilled,frozen,fresh frozen,unripe,slightly ripe,ripe,overripe,dried,naturally dried,artificially dried,heat treated,irradiated"</formula1>
+      <formula1>"air-dried,artificially dried,brined,candied,canned,cured,dried,fermented,freeze-dried,fresh,heat treated,irradiated,jellied,kippered,naturally dried,pasteurized,pickled,raw,shelf stable,sun-dried,ultraviolet light exposed"</formula1>
     </dataValidation>
-    <dataValidation sqref="I2:I1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"chilled,foodsafe chilled,frozen,refrigerated"</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"ripe,overripe,unripe,slightly ripe"</formula1>
+    </dataValidation>
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"field,fresh market,small grocery,supermarket,biobank,unknown,other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -524,7 +581,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,103 +592,118 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>measured_compound</t>
+          <t>component_type</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>measured_compound_value</t>
+          <t>component_type_label</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>measured_compound_unit</t>
+          <t>component_recorded_value</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>measured_compound_denominator_value</t>
+          <t>component_measurement_unit</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>measured_compound_denominator_unit</t>
+          <t>component_data_points_number</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>measured_compound_data_points_number</t>
+          <t>component_record_date</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>measured_compound_record_date</t>
+          <t>component_analysis_date</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>measured_compound_analysis_date</t>
+          <t>component_comment</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>measured_compound_comment</t>
+          <t>component_derivation_type</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>measured_compound_derivation_type</t>
+          <t>component_limit_of_quantitation</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>measured_compound_limit_of_quantitation</t>
+          <t>laboratory_sample_aggregation_minimum_measured_compound_value</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>laboratory_sample_aggregation_minimum_measured_compound_value</t>
+          <t>laboratory_sample_aggregation_maximum_measured_compound_value</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>laboratory_sample_aggregation_maximum_measured_compound_value</t>
+          <t>laboratory_sample_aggregation_median_measured_compound_value</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>laboratory_sample_aggregation_median_measured_compound_value</t>
+          <t>laboratory_sample_aggregation_measured_compound_standard_deviation</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>laboratory_sample_aggregation_measured_compound_standard_deviation</t>
+          <t>analytical_analysis_measurement_protocol_doi</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>analytical_analysis_measurement_protocol_doi</t>
+          <t>analytical_analysis_measurement_method</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>analytical_analysis_measurement_method</t>
+          <t>laboratory_conducting_analytical_analysis</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>laboratory_conducting_analytical_analysis</t>
+          <t>component_quality_control_remeasurement</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_id</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_aliquot_id</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_batch_id</t>
         </is>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="Q2:Q1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"HPLC,GLC,GC,Nephelometry,Gravimetric,Fluorometric,Kjeldahl"</formula1>
     </dataValidation>
   </dataValidations>
@@ -645,7 +717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -656,12 +728,78 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>dataset_label</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mifc_version_tag</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>contributor_orcid</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>organization_name</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_aliquot_id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>laboratory_sample_batch_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>foods</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
           <t>components</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>provenances</t>
         </is>
       </c>
     </row>

</xml_diff>